<commit_message>
Updates to Forms K and L
</commit_message>
<xml_diff>
--- a/K_registo_pessoas/LEGEND_K_registo_pessoas_cduats-media/LEGEND_K_registo_pessoas_cduats.xlsx
+++ b/K_registo_pessoas/LEGEND_K_registo_pessoas_cduats-media/LEGEND_K_registo_pessoas_cduats.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2736" uniqueCount="1277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2745" uniqueCount="1283">
   <si>
     <t>type</t>
   </si>
@@ -3867,14 +3867,39 @@
   <si>
     <t>LEGEND_K_V2</t>
   </si>
+  <si>
+    <t>Abrão Saraiva Namuire</t>
+  </si>
+  <si>
+    <t>Leonardo Pedro Henriques</t>
+  </si>
+  <si>
+    <t>Luis Jacinto Botomane</t>
+  </si>
+  <si>
+    <t>Abrão_Namuire</t>
+  </si>
+  <si>
+    <t>Leonardo_Henriques</t>
+  </si>
+  <si>
+    <t>Luis_Botomane</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -4093,275 +4118,278 @@
   </borders>
   <cellStyleXfs count="237">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -4371,86 +4399,83 @@
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="233" applyFont="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="234" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="234" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="233" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="233" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="233" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="233" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="236" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="236" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="236" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="236" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="236" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="236" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="236" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4459,61 +4484,62 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="233" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="237">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5091,7 +5117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -5769,13 +5795,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C86" sqref="C86"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5822,11 +5848,11 @@
       <c r="A3" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="39" t="s">
-        <v>1176</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>1177</v>
+      <c r="B3" s="40" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C3" s="89" t="s">
+        <v>1277</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="2"/>
@@ -5836,66 +5862,66 @@
       <c r="A4" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="40" t="s">
-        <v>1178</v>
-      </c>
-      <c r="C4" s="41" t="s">
-        <v>1158</v>
+      <c r="B4" s="39" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>1177</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="39" t="s">
-        <v>1179</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>1180</v>
+      <c r="B5" s="40" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>1158</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="40" t="s">
-        <v>1181</v>
-      </c>
-      <c r="C6" s="41" t="s">
-        <v>46</v>
+      <c r="B6" s="39" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>1180</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="39" t="s">
-        <v>1182</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>1183</v>
+      <c r="B7" s="40" t="s">
+        <v>1181</v>
+      </c>
+      <c r="C7" s="41" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="40" t="s">
-        <v>1184</v>
-      </c>
-      <c r="C8" s="41" t="s">
-        <v>1159</v>
+      <c r="B8" s="39" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>1183</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="39" t="s">
-        <v>1185</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>1186</v>
+      <c r="B9" s="40" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>1159</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="17"/>
@@ -5906,11 +5932,11 @@
       <c r="A10" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="39" t="s">
-        <v>1187</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>1188</v>
+      <c r="B10" s="40" t="s">
+        <v>1281</v>
+      </c>
+      <c r="C10" s="89" t="s">
+        <v>1278</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="17"/>
@@ -5921,11 +5947,11 @@
       <c r="A11" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="40" t="s">
-        <v>1189</v>
-      </c>
-      <c r="C11" s="41" t="s">
-        <v>1160</v>
+      <c r="B11" s="39" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>1186</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -5933,10 +5959,10 @@
         <v>18</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>1190</v>
-      </c>
-      <c r="C12" s="41" t="s">
-        <v>1161</v>
+        <v>1282</v>
+      </c>
+      <c r="C12" s="89" t="s">
+        <v>1279</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -5944,10 +5970,10 @@
         <v>18</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>1191</v>
+        <v>1187</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>1162</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -5955,97 +5981,97 @@
         <v>18</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>1192</v>
+        <v>1189</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>1163</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="40" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="C18" s="38" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="11"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="11"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B20" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C20" s="16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B21" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C21" s="16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>49</v>
-      </c>
-    </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>50</v>
-      </c>
+      <c r="A22" s="12"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="4"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="C23" s="29" t="s">
-        <v>114</v>
+      <c r="B23" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -6053,10 +6079,10 @@
         <v>40</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -6064,21 +6090,21 @@
         <v>40</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C26" s="20" t="s">
-        <v>53</v>
+      <c r="B26" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -6086,10 +6112,10 @@
         <v>40</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>42</v>
+        <v>79</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -6097,127 +6123,127 @@
         <v>40</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="24" t="s">
-        <v>84</v>
+      <c r="B29" s="23" t="s">
+        <v>81</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C33" s="9" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="26" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="B33" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="C33" s="26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="26"/>
-      <c r="B34" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="C34" s="26"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="26"/>
+      <c r="B37" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" s="26"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="B36" s="27" t="s">
+      <c r="B38" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="26" t="s">
+      <c r="C39" s="26" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="26" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="B37" s="27" t="s">
+      <c r="B40" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="26" t="s">
+      <c r="C40" s="26" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="B39" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="B40" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="B41" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -6225,10 +6251,10 @@
         <v>111</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -6236,43 +6262,43 @@
         <v>111</v>
       </c>
       <c r="B43" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="B45" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="B46" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C46" s="9" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="B45" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="C45" s="30" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="B46" s="31" t="s">
-        <v>161</v>
-      </c>
-      <c r="C46" s="30" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="30" t="s">
-        <v>140</v>
-      </c>
-      <c r="B47" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="C47" s="30" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -6280,10 +6306,10 @@
         <v>140</v>
       </c>
       <c r="B48" s="31" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C48" s="30" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -6291,10 +6317,10 @@
         <v>140</v>
       </c>
       <c r="B49" s="31" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C49" s="30" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -6302,10 +6328,10 @@
         <v>140</v>
       </c>
       <c r="B50" s="31" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C50" s="30" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -6313,10 +6339,10 @@
         <v>140</v>
       </c>
       <c r="B51" s="31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C51" s="30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -6324,10 +6350,10 @@
         <v>140</v>
       </c>
       <c r="B52" s="31" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C52" s="30" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -6335,10 +6361,10 @@
         <v>140</v>
       </c>
       <c r="B53" s="31" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="C53" s="30" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -6346,10 +6372,10 @@
         <v>140</v>
       </c>
       <c r="B54" s="31" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C54" s="30" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -6357,10 +6383,10 @@
         <v>140</v>
       </c>
       <c r="B55" s="31" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C55" s="30" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -6368,10 +6394,10 @@
         <v>140</v>
       </c>
       <c r="B56" s="31" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="C56" s="30" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -6379,10 +6405,10 @@
         <v>140</v>
       </c>
       <c r="B57" s="31" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C57" s="30" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -6390,10 +6416,10 @@
         <v>140</v>
       </c>
       <c r="B58" s="31" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="C58" s="30" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -6401,10 +6427,10 @@
         <v>140</v>
       </c>
       <c r="B59" s="31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C59" s="30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -6412,10 +6438,10 @@
         <v>140</v>
       </c>
       <c r="B60" s="31" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C60" s="30" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -6423,43 +6449,43 @@
         <v>140</v>
       </c>
       <c r="B61" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="C61" s="30" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="B62" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="C62" s="30" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="B63" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="C63" s="30" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="B64" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="C61" s="30" t="s">
+      <c r="C64" s="30" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="B63" s="36" t="s">
-        <v>203</v>
-      </c>
-      <c r="C63" s="37" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="B64" s="36" t="s">
-        <v>189</v>
-      </c>
-      <c r="C64" s="37" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="B65" s="36" t="s">
-        <v>191</v>
-      </c>
-      <c r="C65" s="37" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -6467,10 +6493,10 @@
         <v>186</v>
       </c>
       <c r="B66" s="36" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="C66" s="37" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -6478,10 +6504,10 @@
         <v>186</v>
       </c>
       <c r="B67" s="36" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C67" s="37" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -6489,10 +6515,10 @@
         <v>186</v>
       </c>
       <c r="B68" s="36" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C68" s="37" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -6500,10 +6526,10 @@
         <v>186</v>
       </c>
       <c r="B69" s="36" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C69" s="37" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -6511,10 +6537,10 @@
         <v>186</v>
       </c>
       <c r="B70" s="36" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C70" s="37" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -6522,10 +6548,10 @@
         <v>186</v>
       </c>
       <c r="B71" s="36" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C71" s="37" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -6533,68 +6559,68 @@
         <v>186</v>
       </c>
       <c r="B72" s="36" t="s">
+        <v>205</v>
+      </c>
+      <c r="C72" s="37" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="B73" s="36" t="s">
+        <v>193</v>
+      </c>
+      <c r="C73" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="B74" s="36" t="s">
+        <v>199</v>
+      </c>
+      <c r="C74" s="37" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="B75" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="C72" s="37" t="s">
+      <c r="C75" s="37" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C74" s="43"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="68" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C77" s="43"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="68" t="s">
         <v>1247</v>
       </c>
-      <c r="B75" s="69" t="s">
+      <c r="B78" s="69" t="s">
         <v>1248</v>
       </c>
-      <c r="C75" s="68" t="s">
+      <c r="C78" s="68" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="68" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="68" t="s">
         <v>1247</v>
       </c>
-      <c r="B76" s="69" t="s">
+      <c r="B79" s="69" t="s">
         <v>1249</v>
       </c>
-      <c r="C76" s="68" t="s">
+      <c r="C79" s="68" t="s">
         <v>1249</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="87" t="s">
-        <v>1261</v>
-      </c>
-      <c r="B78" s="88" t="s">
-        <v>1266</v>
-      </c>
-      <c r="C78" s="87" t="s">
-        <v>1267</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="87" t="s">
-        <v>1261</v>
-      </c>
-      <c r="B79" s="88" t="s">
-        <v>1268</v>
-      </c>
-      <c r="C79" s="87" t="s">
-        <v>1269</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="87" t="s">
-        <v>1261</v>
-      </c>
-      <c r="B80" s="88" t="s">
-        <v>1256</v>
-      </c>
-      <c r="C80" s="87" t="s">
-        <v>1270</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -6602,16 +6628,49 @@
         <v>1261</v>
       </c>
       <c r="B81" s="88" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C81" s="87" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="87" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B82" s="88" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C82" s="87" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="87" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B83" s="88" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C83" s="87" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="87" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B84" s="88" t="s">
         <v>1271</v>
       </c>
-      <c r="C81" s="87" t="s">
+      <c r="C84" s="87" t="s">
         <v>1272</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F11" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <sortState ref="B45:C60">
-    <sortCondition ref="C45:C60"/>
+  <sortState ref="B3:C17">
+    <sortCondition ref="C3:C17"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -31473,8 +31532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31508,7 +31567,7 @@
         <v>1276</v>
       </c>
       <c r="C2" s="32">
-        <v>201710011</v>
+        <v>201712191</v>
       </c>
       <c r="D2" s="67" t="s">
         <v>1246</v>

</xml_diff>